<commit_message>
published working version of multimodal gp service
</commit_message>
<xml_diff>
--- a/PPA3 Troubleshooting Log.xlsx
+++ b/PPA3 Troubleshooting Log.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dconly\GitRepos\PPA3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FEE7A695-8367-479B-BA04-89BA728868DA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6328F0CF-7E3C-4174-A8CC-60261D7F9EA5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="10">
   <si>
     <t>Problem</t>
   </si>
@@ -39,23 +39,31 @@
     <t>ESRI Follow-up?</t>
   </si>
   <si>
-    <t>***Post on GeoNet if problem returns</t>
-  </si>
-  <si>
-    <t>3/1/2022 - Manually copying over the scripts that didn't work onto the server computer seems to fix.</t>
-  </si>
-  <si>
     <t>Diagnosis questions</t>
   </si>
   <si>
     <t>Maybe it only uploads scripts called by the main run script?</t>
+  </si>
+  <si>
+    <t>When publishing, get error 00068 "script XX contains broken project data source: &lt;feature layer name&gt;"</t>
+  </si>
+  <si>
+    <t>Geonet thread</t>
+  </si>
+  <si>
+    <t>3/1/2022 - Manually copying over the scripts that didn't work onto the server computer seems to fix.
+3/6/2022 - Instead of running "from module import function", run "import module.function" or "import module"--this will enable that script to automatically copy over, but the 'utils' folder still doesn't publish, even with an __init__.py in it</t>
+  </si>
+  <si>
+    <t>Generally, try to find and tweak the string that may be causing the issue--usually it's because GIS is trying to confirm if it's a data source, and if it finds it is invalue, it will through the error.
+Workaround: make one offending url string a 1-item list, then pluck it back out of the list once it's being used--that way, ArcGIS thinks it's a list an doesn't scrutinize it like a string.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -67,6 +75,14 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -89,10 +105,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -101,8 +118,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -381,10 +400,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F19" sqref="F19"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -402,28 +421,43 @@
         <v>1</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" ht="90" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>2</v>
       </c>
       <c r="B2" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="D2" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="D2" s="1" t="s">
-        <v>4</v>
+    </row>
+    <row r="3" spans="1:4" ht="120" x14ac:dyDescent="0.25">
+      <c r="A3" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>7</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="D2" r:id="rId1" xr:uid="{8DA3FD34-FE56-402C-97ED-446D228DD2DE}"/>
+    <hyperlink ref="D3" r:id="rId2" xr:uid="{657E0BC2-DE44-4833-8E84-A5A0AF642093}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
+  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
started folder for art agr economy subreport; updated map maker script for freight art exp subreport
</commit_message>
<xml_diff>
--- a/PPA3 Troubleshooting Log.xlsx
+++ b/PPA3 Troubleshooting Log.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24931"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25028"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dconly\GitRepos\PPA3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6328F0CF-7E3C-4174-A8CC-60261D7F9EA5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6DA3D954-6201-4CE0-B1F2-156C5018C0A5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="13">
   <si>
     <t>Problem</t>
   </si>
@@ -57,6 +57,17 @@
   <si>
     <t>Generally, try to find and tweak the string that may be causing the issue--usually it's because GIS is trying to confirm if it's a data source, and if it finds it is invalue, it will through the error.
 Workaround: make one offending url string a 1-item list, then pluck it back out of the list once it's being used--that way, ArcGIS thinks it's a list an doesn't scrutinize it like a string.</t>
+  </si>
+  <si>
+    <t>If GP service isn't restarted every time, then report maps don't reflect the user's line--they only show first line drawn after the GP service was last restarted.</t>
+  </si>
+  <si>
+    <t>Does it affect desktop version? No, works fine on desktop; 
+after running desktop, then running online tool? Online tool works okay.
+Does it only affect multimodal report? No affects all reports, and seems to be "cross report" issue. E.g., submit project in MM report, that project line is in subsequent report even using other tool (e.g. Freight report). Looks like APRX calling issue--problem that all tools calling to same APRX?</t>
+  </si>
+  <si>
+    <t>3/21/2022 - seems intermittent; hard to pin down.</t>
   </si>
 </sst>
 </file>
@@ -400,10 +411,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -452,6 +463,17 @@
         <v>7</v>
       </c>
     </row>
+    <row r="4" spans="1:4" ht="150" x14ac:dyDescent="0.25">
+      <c r="A4" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="D2" r:id="rId1" xr:uid="{8DA3FD34-FE56-402C-97ED-446D228DD2DE}"/>

</xml_diff>

<commit_message>
initial art sgr sgr report; added backups of JSON files used
</commit_message>
<xml_diff>
--- a/PPA3 Troubleshooting Log.xlsx
+++ b/PPA3 Troubleshooting Log.xlsx
@@ -8,17 +8,27 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dconly\GitRepos\PPA3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6DA3D954-6201-4CE0-B1F2-156C5018C0A5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CBEF712A-DBD9-497E-A14C-0CAEEEC53E83}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -414,7 +424,7 @@
   <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
added to troubleshooting log
</commit_message>
<xml_diff>
--- a/PPA3 Troubleshooting Log.xlsx
+++ b/PPA3 Troubleshooting Log.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dconly\GitRepos\PPA3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CBEF712A-DBD9-497E-A14C-0CAEEEC53E83}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE5BA70E-7117-4935-B760-72F71CF9EA50}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="17">
   <si>
     <t>Problem</t>
   </si>
@@ -63,10 +63,6 @@
   <si>
     <t>3/1/2022 - Manually copying over the scripts that didn't work onto the server computer seems to fix.
 3/6/2022 - Instead of running "from module import function", run "import module.function" or "import module"--this will enable that script to automatically copy over, but the 'utils' folder still doesn't publish, even with an __init__.py in it</t>
-  </si>
-  <si>
-    <t>Generally, try to find and tweak the string that may be causing the issue--usually it's because GIS is trying to confirm if it's a data source, and if it finds it is invalue, it will through the error.
-Workaround: make one offending url string a 1-item list, then pluck it back out of the list once it's being used--that way, ArcGIS thinks it's a list an doesn't scrutinize it like a string.</t>
   </si>
   <si>
     <t>If GP service isn't restarted every time, then report maps don't reflect the user's line--they only show first line drawn after the GP service was last restarted.</t>
@@ -78,6 +74,22 @@
   </si>
   <si>
     <t>3/21/2022 - seems intermittent; hard to pin down.</t>
+  </si>
+  <si>
+    <t>Generally, try to find and tweak the string that may be causing the issue--usually it's because GIS is trying to confirm if it's a data source, and if it finds it is invalid it will through the error.
+Workaround: make one offending url string a 1-item list, then pluck it back out of the list once it's being used--that way, ArcGIS thinks it's a list an doesn't scrutinize it like a string.</t>
+  </si>
+  <si>
+    <t>Geonet thread DC posted 3/31/2022</t>
+  </si>
+  <si>
+    <t>000358: Invalid expression when running select-by-attributes command in arcpy</t>
+  </si>
+  <si>
+    <t>If it happens when running in Arc Pro, make sure that none of the columns are hidden for the layer that the selection is happening on.</t>
+  </si>
+  <si>
+    <t>NA</t>
   </si>
 </sst>
 </file>
@@ -130,7 +142,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -140,6 +152,9 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -421,10 +436,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -462,12 +477,12 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="120" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" ht="105" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>6</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="D3" s="4" t="s">
         <v>7</v>
@@ -475,21 +490,39 @@
     </row>
     <row r="4" spans="1:4" ht="150" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="B4" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>11</v>
+      <c r="D4" s="5" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A5" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D5" t="s">
+        <v>16</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="D2" r:id="rId1" xr:uid="{8DA3FD34-FE56-402C-97ED-446D228DD2DE}"/>
     <hyperlink ref="D3" r:id="rId2" xr:uid="{657E0BC2-DE44-4833-8E84-A5A0AF642093}"/>
+    <hyperlink ref="D4" r:id="rId3" xr:uid="{32E1D8BA-E56F-4998-816D-EF48A81AB537}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId3"/>
+  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId4"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
in fwy econ report map maker script, run DeleteFeatures on feature layer of line template instead of feature class--might help with map stickage problem
</commit_message>
<xml_diff>
--- a/PPA3 Troubleshooting Log.xlsx
+++ b/PPA3 Troubleshooting Log.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dconly\GitRepos\PPA3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE5BA70E-7117-4935-B760-72F71CF9EA50}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59AC0F85-3DA2-43CF-ADFB-DA5FC6CC8F28}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="15600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -73,9 +73,6 @@
 Does it only affect multimodal report? No affects all reports, and seems to be "cross report" issue. E.g., submit project in MM report, that project line is in subsequent report even using other tool (e.g. Freight report). Looks like APRX calling issue--problem that all tools calling to same APRX?</t>
   </si>
   <si>
-    <t>3/21/2022 - seems intermittent; hard to pin down.</t>
-  </si>
-  <si>
     <t>Generally, try to find and tweak the string that may be causing the issue--usually it's because GIS is trying to confirm if it's a data source, and if it finds it is invalid it will through the error.
 Workaround: make one offending url string a 1-item list, then pluck it back out of the list once it's being used--that way, ArcGIS thinks it's a list an doesn't scrutinize it like a string.</t>
   </si>
@@ -90,6 +87,10 @@
   </si>
   <si>
     <t>NA</t>
+  </si>
+  <si>
+    <t>3/21/2022 - seems intermittent; hard to pin down.
+4/4/2022 - for one report (fwy econ prosperity), running DeleteFeatures on feature layer instead of feature class seems to fix it, but on other reports the issue doesn't seem to be cropping up.</t>
   </si>
 </sst>
 </file>
@@ -482,7 +483,7 @@
         <v>6</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D3" s="4" t="s">
         <v>7</v>
@@ -493,27 +494,27 @@
         <v>9</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="C4" s="3" t="s">
         <v>10</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B5" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="B5" s="3" t="s">
+      <c r="C5" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="C5" s="3" t="s">
-        <v>16</v>
-      </c>
       <c r="D5" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
   </sheetData>

</xml_diff>